<commit_message>
Ajout de code pour export
</commit_message>
<xml_diff>
--- a/data_output.xlsx
+++ b/data_output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ENCAISSEMENT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +25,25 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +51,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,104 +440,104 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Intitulé</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>year</t>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>25/04/2024</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Cumul Mois</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cumul Année</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Chèques</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" s="3" t="n">
+        <v>580048.29</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>580048.29</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Coupon</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3" s="3" t="n">
+        <v>21742.39</v>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>21742.39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Espèces</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="3" t="n">
         <v>79841.64</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4" s="3" t="n">
+        <v>5043137.91</v>
+      </c>
+      <c r="D4" s="3" t="n">
         <v>5043137.91</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Mvola</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" s="3" t="n">
+        <v>151987.06</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>151987.06</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>TPE</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" s="3" t="n">
+        <v>242367.05</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>242367.05</v>
       </c>
     </row>

</xml_diff>